<commit_message>
- Changed DeepSleep handling. - Modified Firebase parameters handling Deep Sleep - Added time adjustment to danish summertime (permanently). - Added power down of sensor unit during setup() - Changed schematics and wrap layout of hardware - added some loose power calculations of solar charging - some general clean-up (non functional)
</commit_message>
<xml_diff>
--- a/docs/Solar Opladere.xlsx
+++ b/docs/Solar Opladere.xlsx
@@ -1,22 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\_SRC\projects\Vanding\AutoIrrigation\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63DB0FE-7AA5-4A3F-AC68-E2CE9D0DD4F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12330"/>
+    <workbookView xWindow="-15870" yWindow="-1725" windowWidth="15990" windowHeight="24990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="behov" sheetId="2" r:id="rId1"/>
+    <sheet name="opladere" sheetId="1" r:id="rId2"/>
+    <sheet name="solpaneler" sheetId="3" r:id="rId3"/>
+    <sheet name="vinkel og placering" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>http://www.scosche.com/consumer-tech/product/2073</t>
   </si>
@@ -133,12 +148,84 @@
   </si>
   <si>
     <t>16.5 x 14.5 x 4 cm</t>
+  </si>
+  <si>
+    <t>eff. battery capacity
+[mAh @ 3.7V]</t>
+  </si>
+  <si>
+    <t>Hours to charge fully</t>
+  </si>
+  <si>
+    <t>Days @ 6h/day</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Nom. Cap. [V]</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>max mA</t>
+  </si>
+  <si>
+    <t>Max power [W]</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/ANBES-Solar-Panel-5V-6V-12V-Mini-Solar-System-DIY-For-Battery-Cell-Phone-Chargers-Portable/32848710253.html</t>
+  </si>
+  <si>
+    <t>Daily sun hours</t>
+  </si>
+  <si>
+    <t>wH / day</t>
+  </si>
+  <si>
+    <t>output [mA]
+DIRECT sun</t>
+  </si>
+  <si>
+    <t>output [mA]
+INDIRECT sun</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>Rated max [V]</t>
+  </si>
+  <si>
+    <t>Ratex max [W]</t>
+  </si>
+  <si>
+    <t>output [W]</t>
+  </si>
+  <si>
+    <t>110x69</t>
+  </si>
+  <si>
+    <t>https://sinovoltaics.com/learning-center/system-design/solar-panel-angle-tilt-calculation/</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Summer factor</t>
+  </si>
+  <si>
+    <t>Best angle (summer)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -208,6 +295,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -218,6 +308,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -266,7 +359,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,9 +392,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -334,6 +444,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,10 +636,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A4:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>0.8*3600</f>
+        <v>2880</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1.25</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <f>F5*3.7/1000</f>
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H5">
+        <f>A5/F5</f>
+        <v>576</v>
+      </c>
+      <c r="I5">
+        <f>H5/6</f>
+        <v>96</v>
+      </c>
+      <c r="J5">
+        <v>150</v>
+      </c>
+      <c r="K5">
+        <f>J5*3.7/1000</f>
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="L5">
+        <f>A5/J5</f>
+        <v>19.2</v>
+      </c>
+      <c r="M5">
+        <f>L5/6</f>
+        <v>3.1999999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -755,38 +989,165 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6" display="http://www.mytrendyphone.dk/shop/a-solar-al-260-power-73510p.html?utm_source=feed-kelkoo_dk&amp;utm_medium=feed&amp;utm_campaign=feed-kelkoo_dk&amp;network=KELKOODA&amp;utm_source=kelkoodk&amp;utm_medium=cpc&amp;utm_campaign=kelkooclick&amp;utm_term=A-Solar%20AL-260%20Power%20Bank%20Oplader&amp;sstlcmpid=9433"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="http://www.mytrendyphone.dk/shop/a-solar-al-260-power-73510p.html?utm_source=feed-kelkoo_dk&amp;utm_medium=feed&amp;utm_campaign=feed-kelkoo_dk&amp;network=KELKOODA&amp;utm_source=kelkoodk&amp;utm_medium=cpc&amp;utm_campaign=kelkooclick&amp;utm_term=A-Solar%20AL-260%20Power%20Bank%20Oplader&amp;sstlcmpid=9433" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0.6</v>
+      </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
+      <c r="E2">
+        <v>55</v>
+      </c>
+      <c r="G2">
+        <f>C2*$T$1*0.75</f>
+        <v>2.6999999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0.6</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+      <c r="E3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1.25</v>
+      </c>
+      <c r="D4">
+        <v>110</v>
+      </c>
+      <c r="E4">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6613C702-0D8E-49A3-826E-4BB89B6A8243}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5490FA1B-0374-4DD3-9AE3-12B245E2DE0F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159F82DF-88E9-426D-B8B6-49E3740FFF4B}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>55.676098000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>-23.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <f>(B3*0.9)+B4</f>
+        <v>26.608488200000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{30FED8C5-F163-4452-99E2-10BBA46A7979}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>